<commit_message>
Update list of disease
</commit_message>
<xml_diff>
--- a/Source Code/Store Procedure and Functions/Meta data/Speciality and Disease.xlsx
+++ b/Source Code/Store Procedure and Functions/Meta data/Speciality and Disease.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Speciality" sheetId="21" r:id="rId1"/>
@@ -34,6 +34,8 @@
     <sheet name="THÂN-NIỆU HỌC" sheetId="11" r:id="rId20"/>
     <sheet name="THẬN NỘI TIẾT" sheetId="1" r:id="rId21"/>
     <sheet name="UNG BƯỚU" sheetId="5" r:id="rId22"/>
+    <sheet name="CƠ XƯƠNG KHỚP" sheetId="23" r:id="rId23"/>
+    <sheet name="Y HỌC CỔ TRUYỀN" sheetId="24" r:id="rId24"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="1507">
   <si>
     <t>(N'Abces gan'), -- Tiêu hóa</t>
   </si>
@@ -4293,13 +4295,286 @@
   </si>
   <si>
     <t>Vú tăng sản không điển hình</t>
+  </si>
+  <si>
+    <t>(N'Trật khớp'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy xương'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Trật khớp khuỷu'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Sai khớp vai'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Sai khớp háng'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy đầu trên xương cẳng tay'), --CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy đầu dưới xương cẳng tay'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy khung chậu'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy xương bánh chè'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy thân xương đùi'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy cổ xương đùi'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy thân xương cẳng tay'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy thân xương cẳng chân'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gãy xương bả vai'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Bệnh giả Gout'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Bệnh Paget xương'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gout'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Gai xương'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Đau cổ'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Đau đầu gối'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Đau lưng'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Loãng xương'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Rách dây chằng trước khớp gối'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Thoát vị đĩa đệm'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Ung thư xương'), -- CƠ XƯƠNG KHỚP,UNG BƯỚU</t>
+  </si>
+  <si>
+    <t>(N'Viêm bao hoạt dịch'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Viêm gân'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Viêm gân bánh chè'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Viêm khớp'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Viêm khớp nhiễm khuẩn'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Viêm khớp phản ứng'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Viêm khớp vẩy nến'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Viêm xương tủy'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Vô mạch hoại tử'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Vỡ xương mắt cá chân'), -- CƠ XƯƠNG KHỚP</t>
+  </si>
+  <si>
+    <t>(N'Đởm lạc kết thạch'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Đởm lạc cảm nhiễm'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Động kinh'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Đau thần kinh tọa'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Xơ mỡ động mạch'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Xơ gan'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm đại tràng mạn'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm tiểu cầu thận mãn tính'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm thận, tiểu cầu cấp tính'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm teo niêm mạc dạ dày mãn tính hay thoái hóa niêm mạc dạ dày'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm sinh dục nữ'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm phế quản cấp, mạn'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm não màng não lưu hành tính'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm não -tủy cấp'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm khớp phong thấp tính'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm gan mạn tính hoạt động'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Viêm gan mạn'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Vị nham'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Cổ tử cung nham'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Tiết niệu kết thạch'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Tiết niệu lạc cảm nhiễm'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>(N'Tim mạch và phong thấp nhiệt tính'), -- Y HỌC CỔ TRUYỀN</t>
+  </si>
+  <si>
+    <t>Trật khớp</t>
+  </si>
+  <si>
+    <t>Gãy xương</t>
+  </si>
+  <si>
+    <t>Trật khớp khuỷu</t>
+  </si>
+  <si>
+    <t>Sai khớp vai</t>
+  </si>
+  <si>
+    <t>Sai khớp háng</t>
+  </si>
+  <si>
+    <t>Gãy đầu trên xương cẳng tay</t>
+  </si>
+  <si>
+    <t>Gãy đầu dưới xương cẳng tay</t>
+  </si>
+  <si>
+    <t>Gãy khung chậu</t>
+  </si>
+  <si>
+    <t>Gãy xương bánh chè</t>
+  </si>
+  <si>
+    <t>Gãy thân xương đùi</t>
+  </si>
+  <si>
+    <t>Gãy cổ xương đùi</t>
+  </si>
+  <si>
+    <t>Gãy thân xương cẳng tay</t>
+  </si>
+  <si>
+    <t>Gãy thân xương cẳng chân</t>
+  </si>
+  <si>
+    <t>Gãy xương bả vai</t>
+  </si>
+  <si>
+    <t>Viêm khớp nhiễm khuẩn</t>
+  </si>
+  <si>
+    <t>Đởm lạc kết thạch</t>
+  </si>
+  <si>
+    <t>Đởm lạc cảm nhiễm</t>
+  </si>
+  <si>
+    <t>Đau thần kinh tọa</t>
+  </si>
+  <si>
+    <t>Xơ mỡ động mạch</t>
+  </si>
+  <si>
+    <t>Viêm đại tràng mạn</t>
+  </si>
+  <si>
+    <t>Viêm tiểu cầu thận mãn tính</t>
+  </si>
+  <si>
+    <t>Viêm thận, tiểu cầu cấp tính</t>
+  </si>
+  <si>
+    <t>Viêm teo niêm mạc dạ dày mãn tính hay thoái hóa niêm mạc dạ dày</t>
+  </si>
+  <si>
+    <t>Viêm sinh dục nữ</t>
+  </si>
+  <si>
+    <t>Viêm phế quản cấp, mạn</t>
+  </si>
+  <si>
+    <t>Viêm não màng não lưu hành tính</t>
+  </si>
+  <si>
+    <t>Viêm não -tủy cấp</t>
+  </si>
+  <si>
+    <t>Viêm khớp phong thấp tính</t>
+  </si>
+  <si>
+    <t>Viêm gan mạn tính hoạt động</t>
+  </si>
+  <si>
+    <t>Vị nham</t>
+  </si>
+  <si>
+    <t>Cổ tử cung nham</t>
+  </si>
+  <si>
+    <t>Tiết niệu kết thạch</t>
+  </si>
+  <si>
+    <t>Tiết niệu lạc cảm nhiễm</t>
+  </si>
+  <si>
+    <t>Tim mạch và phong thấp nhiệt tính</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4311,6 +4586,14 @@
       <b/>
       <sz val="14"/>
       <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4489,7 +4772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -4536,6 +4819,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4818,7 +5102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7624,9 +7908,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C707"/>
+  <dimension ref="A1:C764"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15401,19 +15685,647 @@
         <v>1</v>
       </c>
     </row>
-    <row r="707" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A707" s="19">
+    <row r="707" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A707" s="16">
         <v>706</v>
       </c>
-      <c r="B707" s="20" t="s">
+      <c r="B707" s="17" t="s">
         <v>1204</v>
       </c>
-      <c r="C707" s="21">
+      <c r="C707" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="708" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A708" s="16">
+        <v>707</v>
+      </c>
+      <c r="B708" s="17" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C708" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="709" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A709" s="16">
+        <v>708</v>
+      </c>
+      <c r="B709" s="17" t="s">
+        <v>1474</v>
+      </c>
+      <c r="C709" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="710" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A710" s="16">
+        <v>709</v>
+      </c>
+      <c r="B710" s="17" t="s">
+        <v>1475</v>
+      </c>
+      <c r="C710" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="711" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A711" s="16">
+        <v>710</v>
+      </c>
+      <c r="B711" s="17" t="s">
+        <v>1476</v>
+      </c>
+      <c r="C711" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="712" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A712" s="16">
+        <v>711</v>
+      </c>
+      <c r="B712" s="17" t="s">
+        <v>1477</v>
+      </c>
+      <c r="C712" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="713" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A713" s="16">
+        <v>712</v>
+      </c>
+      <c r="B713" s="17" t="s">
+        <v>1478</v>
+      </c>
+      <c r="C713" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="714" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A714" s="16">
+        <v>713</v>
+      </c>
+      <c r="B714" s="17" t="s">
+        <v>1479</v>
+      </c>
+      <c r="C714" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="715" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A715" s="16">
+        <v>714</v>
+      </c>
+      <c r="B715" s="17" t="s">
+        <v>1480</v>
+      </c>
+      <c r="C715" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="716" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A716" s="16">
+        <v>715</v>
+      </c>
+      <c r="B716" s="17" t="s">
+        <v>1481</v>
+      </c>
+      <c r="C716" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="717" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A717" s="16">
+        <v>716</v>
+      </c>
+      <c r="B717" s="17" t="s">
+        <v>1482</v>
+      </c>
+      <c r="C717" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="718" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A718" s="16">
+        <v>717</v>
+      </c>
+      <c r="B718" s="17" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C718" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="719" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A719" s="16">
+        <v>718</v>
+      </c>
+      <c r="B719" s="17" t="s">
+        <v>1484</v>
+      </c>
+      <c r="C719" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="720" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A720" s="16">
+        <v>719</v>
+      </c>
+      <c r="B720" s="17" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C720" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="721" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A721" s="16">
+        <v>720</v>
+      </c>
+      <c r="B721" s="17" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C721" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="722" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A722" s="16">
+        <v>721</v>
+      </c>
+      <c r="B722" s="17" t="s">
+        <v>742</v>
+      </c>
+      <c r="C722" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="723" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A723" s="16">
+        <v>722</v>
+      </c>
+      <c r="B723" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C723" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="724" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A724" s="16">
+        <v>723</v>
+      </c>
+      <c r="B724" s="17" t="s">
+        <v>748</v>
+      </c>
+      <c r="C724" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="725" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A725" s="16">
+        <v>724</v>
+      </c>
+      <c r="B725" s="17" t="s">
+        <v>747</v>
+      </c>
+      <c r="C725" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="726" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A726" s="16">
+        <v>725</v>
+      </c>
+      <c r="B726" s="17" t="s">
+        <v>744</v>
+      </c>
+      <c r="C726" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="727" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A727" s="16">
+        <v>726</v>
+      </c>
+      <c r="B727" s="17" t="s">
+        <v>745</v>
+      </c>
+      <c r="C727" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="728" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A728" s="16">
+        <v>727</v>
+      </c>
+      <c r="B728" s="17" t="s">
+        <v>746</v>
+      </c>
+      <c r="C728" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="729" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A729" s="16">
+        <v>728</v>
+      </c>
+      <c r="B729" s="17" t="s">
+        <v>750</v>
+      </c>
+      <c r="C729" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="730" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A730" s="16">
+        <v>729</v>
+      </c>
+      <c r="B730" s="17" t="s">
+        <v>752</v>
+      </c>
+      <c r="C730" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="731" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A731" s="16">
+        <v>730</v>
+      </c>
+      <c r="B731" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="C731" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="732" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A732" s="16">
+        <v>731</v>
+      </c>
+      <c r="B732" s="17" t="s">
+        <v>754</v>
+      </c>
+      <c r="C732" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="733" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A733" s="16">
+        <v>732</v>
+      </c>
+      <c r="B733" s="17" t="s">
+        <v>755</v>
+      </c>
+      <c r="C733" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="734" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A734" s="16">
+        <v>733</v>
+      </c>
+      <c r="B734" s="17" t="s">
+        <v>757</v>
+      </c>
+      <c r="C734" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="735" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A735" s="16">
+        <v>734</v>
+      </c>
+      <c r="B735" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="C735" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="736" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A736" s="16">
+        <v>735</v>
+      </c>
+      <c r="B736" s="17" t="s">
+        <v>759</v>
+      </c>
+      <c r="C736" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="737" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A737" s="16">
+        <v>736</v>
+      </c>
+      <c r="B737" s="17" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C737" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="738" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A738" s="16">
+        <v>737</v>
+      </c>
+      <c r="B738" s="17" t="s">
+        <v>763</v>
+      </c>
+      <c r="C738" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="739" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A739" s="16">
+        <v>738</v>
+      </c>
+      <c r="B739" s="17" t="s">
+        <v>764</v>
+      </c>
+      <c r="C739" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="740" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A740" s="16">
+        <v>739</v>
+      </c>
+      <c r="B740" s="17" t="s">
+        <v>766</v>
+      </c>
+      <c r="C740" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="741" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A741" s="16">
+        <v>740</v>
+      </c>
+      <c r="B741" s="17" t="s">
+        <v>767</v>
+      </c>
+      <c r="C741" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="742" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A742" s="16">
+        <v>741</v>
+      </c>
+      <c r="B742" s="17" t="s">
+        <v>768</v>
+      </c>
+      <c r="C742" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="743" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A743" s="16">
+        <v>742</v>
+      </c>
+      <c r="B743" s="17" t="s">
+        <v>1488</v>
+      </c>
+      <c r="C743" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="744" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A744" s="16">
+        <v>743</v>
+      </c>
+      <c r="B744" s="17" t="s">
+        <v>1489</v>
+      </c>
+      <c r="C744" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="745" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A745" s="16">
+        <v>744</v>
+      </c>
+      <c r="B745" s="17" t="s">
+        <v>1310</v>
+      </c>
+      <c r="C745" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="746" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A746" s="16">
+        <v>745</v>
+      </c>
+      <c r="B746" s="17" t="s">
+        <v>1490</v>
+      </c>
+      <c r="C746" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="747" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A747" s="16">
+        <v>746</v>
+      </c>
+      <c r="B747" s="17" t="s">
+        <v>1491</v>
+      </c>
+      <c r="C747" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="748" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A748" s="16">
+        <v>747</v>
+      </c>
+      <c r="B748" s="17" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C748" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="749" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A749" s="16">
+        <v>748</v>
+      </c>
+      <c r="B749" s="17" t="s">
+        <v>1492</v>
+      </c>
+      <c r="C749" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="750" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A750" s="16">
+        <v>749</v>
+      </c>
+      <c r="B750" s="17" t="s">
+        <v>1493</v>
+      </c>
+      <c r="C750" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="751" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A751" s="16">
+        <v>750</v>
+      </c>
+      <c r="B751" s="17" t="s">
+        <v>1494</v>
+      </c>
+      <c r="C751" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="752" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A752" s="16">
+        <v>751</v>
+      </c>
+      <c r="B752" s="17" t="s">
+        <v>1495</v>
+      </c>
+      <c r="C752" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="753" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A753" s="16">
+        <v>752</v>
+      </c>
+      <c r="B753" s="17" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C753" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="754" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A754" s="16">
+        <v>753</v>
+      </c>
+      <c r="B754" s="17" t="s">
+        <v>1497</v>
+      </c>
+      <c r="C754" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="755" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A755" s="16">
+        <v>754</v>
+      </c>
+      <c r="B755" s="17" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C755" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="756" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A756" s="16">
+        <v>755</v>
+      </c>
+      <c r="B756" s="17" t="s">
+        <v>1499</v>
+      </c>
+      <c r="C756" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="757" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A757" s="16">
+        <v>756</v>
+      </c>
+      <c r="B757" s="17" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C757" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="758" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A758" s="16">
+        <v>757</v>
+      </c>
+      <c r="B758" s="17" t="s">
+        <v>1501</v>
+      </c>
+      <c r="C758" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="759" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A759" s="16">
+        <v>758</v>
+      </c>
+      <c r="B759" s="17" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C759" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="760" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A760" s="16">
+        <v>759</v>
+      </c>
+      <c r="B760" s="17" t="s">
+        <v>1502</v>
+      </c>
+      <c r="C760" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="761" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A761" s="16">
+        <v>760</v>
+      </c>
+      <c r="B761" s="17" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C761" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="762" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A762" s="16">
+        <v>761</v>
+      </c>
+      <c r="B762" s="17" t="s">
+        <v>1504</v>
+      </c>
+      <c r="C762" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="763" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A763" s="16">
+        <v>762</v>
+      </c>
+      <c r="B763" s="17" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C763" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="764" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A764" s="19">
+        <v>763</v>
+      </c>
+      <c r="B764" s="20" t="s">
+        <v>1506</v>
+      </c>
+      <c r="C764" s="21">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15764,6 +16676,328 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C10" s="22"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1048576"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>1453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>1465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>1469</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1048576" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>

</xml_diff>